<commit_message>
special sevev was fixed
</commit_message>
<xml_diff>
--- a/תורנים.xlsx
+++ b/תורנים.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\toranim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8F18FD-BEFB-4C8A-AC0F-C8DA0E6A0524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D88D8C-C50B-48C2-90F9-A3932FBF612D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="154">
   <si>
     <t>שם</t>
   </si>
@@ -737,7 +737,7 @@
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
+      <selection pane="bottomLeft" activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1069,10 +1069,10 @@
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="G16" t="s">
-        <v>47</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1089,10 +1089,10 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="G17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1109,10 +1109,10 @@
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1129,10 +1129,10 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1149,10 +1149,10 @@
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>125</v>
+        <v>42</v>
       </c>
       <c r="G20" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1169,10 +1169,10 @@
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>45</v>
+        <v>125</v>
       </c>
       <c r="G21" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1189,10 +1189,10 @@
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1209,10 +1209,10 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="G23" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1229,10 +1229,10 @@
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1249,10 +1249,10 @@
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1269,10 +1269,10 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G26" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1289,10 +1289,10 @@
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="G27" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1309,10 +1309,10 @@
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="G28" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1329,10 +1329,10 @@
         <v>0</v>
       </c>
       <c r="F29" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="G29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1349,10 +1349,10 @@
         <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="G30" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1369,10 +1369,10 @@
         <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G31" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1389,10 +1389,10 @@
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G32" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1409,10 +1409,10 @@
         <v>0</v>
       </c>
       <c r="F33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G33" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1429,10 +1429,10 @@
         <v>0</v>
       </c>
       <c r="F34" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="G34" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1449,10 +1449,10 @@
         <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="G35" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1469,10 +1469,10 @@
         <v>0</v>
       </c>
       <c r="F36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G36" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1489,10 +1489,10 @@
         <v>0</v>
       </c>
       <c r="F37" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G37" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1509,10 +1509,10 @@
         <v>0</v>
       </c>
       <c r="F38" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G38" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1529,10 +1529,10 @@
         <v>0</v>
       </c>
       <c r="F39" t="s">
-        <v>128</v>
+        <v>91</v>
       </c>
       <c r="G39" t="s">
-        <v>26</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1549,10 +1549,10 @@
         <v>0</v>
       </c>
       <c r="F40" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="G40" t="s">
-        <v>95</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1569,10 +1569,10 @@
         <v>1</v>
       </c>
       <c r="F41" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G41" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1589,10 +1589,10 @@
         <v>0</v>
       </c>
       <c r="F42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G42" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1609,10 +1609,10 @@
         <v>0</v>
       </c>
       <c r="F43" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="G43" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1629,10 +1629,10 @@
         <v>0</v>
       </c>
       <c r="F44" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G44" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1649,10 +1649,10 @@
         <v>0</v>
       </c>
       <c r="F45" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G45" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1669,10 +1669,10 @@
         <v>0</v>
       </c>
       <c r="F46" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="G46" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1689,10 +1689,10 @@
         <v>0</v>
       </c>
       <c r="F47" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G47" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1709,10 +1709,10 @@
         <v>0</v>
       </c>
       <c r="F48" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G48" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1729,10 +1729,10 @@
         <v>0</v>
       </c>
       <c r="F49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G49" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1749,10 +1749,10 @@
         <v>0</v>
       </c>
       <c r="F50" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G50" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1769,10 +1769,10 @@
         <v>1</v>
       </c>
       <c r="F51" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="G51" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1789,10 +1789,10 @@
         <v>0</v>
       </c>
       <c r="F52" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="G52" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1809,10 +1809,10 @@
         <v>0</v>
       </c>
       <c r="F53" t="s">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="G53" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1829,10 +1829,10 @@
         <v>0</v>
       </c>
       <c r="F54" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G54" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1849,10 +1849,10 @@
         <v>0</v>
       </c>
       <c r="F55" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="G55" t="s">
-        <v>5</v>
+        <v>122</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1867,6 +1867,12 @@
       </c>
       <c r="D56">
         <v>0</v>
+      </c>
+      <c r="F56" t="s">
+        <v>123</v>
+      </c>
+      <c r="G56" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4018,7 +4024,7 @@
     <row r="981" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F56:G368 F2:G3 F4:G55" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F23:G368 F2:G22" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$2:$A$300</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>